<commit_message>
small updates, reconfig for rivanna/slurm
</commit_message>
<xml_diff>
--- a/data/auxotrophies_references.xlsx
+++ b/data/auxotrophies_references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maureencarey/local_documents/work/comparative_parasite_models/paradigm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEBDF53-07ED-4D4C-BF43-C26B88E7BC6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87203E53-8823-2D46-9035-0A22E58ED39A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="243">
   <si>
     <t>Metabolite</t>
   </si>
@@ -679,13 +679,88 @@
   </si>
   <si>
     <t>pyruvate</t>
+  </si>
+  <si>
+    <t>Leishmania</t>
+  </si>
+  <si>
+    <t>mexicana</t>
+  </si>
+  <si>
+    <t>biochem_uptake: 10.1074/jbc.M110.213553</t>
+  </si>
+  <si>
+    <t>biochem_prod: 10.1074/jbc.M110.213553</t>
+  </si>
+  <si>
+    <t>both: 10.1074/jbc.M110.213553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trypanosoma </t>
+  </si>
+  <si>
+    <t>brucei</t>
+  </si>
+  <si>
+    <t>biochem_uptake: 10.1021/ac3018795</t>
+  </si>
+  <si>
+    <t>biochem_prod: 10.1021/ac3018795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entamoeba </t>
+  </si>
+  <si>
+    <t>histolytica</t>
+  </si>
+  <si>
+    <t>biochem_prod: 10.1371/journal.pntd.0001831</t>
+  </si>
+  <si>
+    <t>methionine sulfoxide</t>
+  </si>
+  <si>
+    <t>acetyl-glucosamine 1-phosphate</t>
+  </si>
+  <si>
+    <t>acetyl-glucosamine 6-phosphate</t>
+  </si>
+  <si>
+    <t>nicotinate</t>
+  </si>
+  <si>
+    <t>phosphoserine</t>
+  </si>
+  <si>
+    <t>sedoheptulose 7-phosphate</t>
+  </si>
+  <si>
+    <t>amp</t>
+  </si>
+  <si>
+    <t>fructose 6-phosphate</t>
+  </si>
+  <si>
+    <t>glycerol 3-phosphate</t>
+  </si>
+  <si>
+    <t>glucose 1-phosphate</t>
+  </si>
+  <si>
+    <t>glucose 6-phosphate</t>
+  </si>
+  <si>
+    <t>phosphoglycerate</t>
+  </si>
+  <si>
+    <t>Dihydroxyacetone phosphate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -766,6 +841,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -788,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -800,6 +882,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1115,18 +1198,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI99"/>
+  <dimension ref="A1:AJ112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AO17" sqref="AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="4.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="3.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="2.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="2.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="4.1640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="2.1640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="3.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="4" style="1" customWidth="1"/>
+    <col min="27" max="28" width="4.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="4.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="4.33203125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="3.83203125" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1226,8 +1338,17 @@
       <c r="AG1" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AH1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -1327,8 +1448,17 @@
       <c r="AG2" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AH2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1371,8 +1501,14 @@
       <c r="AG3" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AH3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
@@ -1391,7 +1527,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -1404,8 +1540,11 @@
       <c r="J5" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AI5" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -1423,8 +1562,14 @@
       <c r="AF6" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AH6" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -1441,7 +1586,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
@@ -1459,8 +1604,11 @@
       <c r="AF8" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AH8" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
@@ -1478,8 +1626,11 @@
       <c r="AF9" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AH9" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>62</v>
       </c>
@@ -1493,7 +1644,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1507,7 +1658,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
@@ -1524,7 +1675,7 @@
       </c>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -1541,7 +1692,7 @@
       </c>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -1555,7 +1706,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -1569,7 +1720,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -1583,7 +1734,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -1596,8 +1747,11 @@
       <c r="J17" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AH17" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -1614,7 +1768,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1627,8 +1781,11 @@
       <c r="J19" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AI19" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -1644,8 +1801,11 @@
       <c r="AF20" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ20" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -1659,7 +1819,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1676,7 +1836,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
@@ -1690,7 +1850,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
@@ -1701,7 +1861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1712,7 +1872,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -1729,7 +1889,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
@@ -1746,7 +1906,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -1754,7 +1914,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
@@ -1765,7 +1925,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1776,15 +1936,18 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ31" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -1792,7 +1955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
@@ -1802,8 +1965,11 @@
       <c r="O33" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AI33" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1811,7 +1977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
@@ -1831,7 +1997,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1848,7 +2014,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>64</v>
       </c>
@@ -1856,7 +2022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -1864,7 +2030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -1872,7 +2038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -1880,7 +2046,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -1888,7 +2054,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1896,7 +2062,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
@@ -1916,7 +2082,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1933,7 +2099,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
@@ -1950,7 +2116,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>65</v>
       </c>
@@ -1967,7 +2133,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>64</v>
       </c>
@@ -1975,7 +2141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>65</v>
       </c>
@@ -1986,7 +2152,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
@@ -1997,7 +2163,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>65</v>
       </c>
@@ -2005,7 +2171,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>64</v>
       </c>
@@ -2013,7 +2179,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -2024,7 +2190,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>66</v>
       </c>
@@ -2035,7 +2201,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>64</v>
       </c>
@@ -2043,7 +2209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
@@ -2054,7 +2220,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>67</v>
       </c>
@@ -2065,7 +2231,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
@@ -2079,7 +2245,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>64</v>
       </c>
@@ -2087,7 +2253,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -2098,7 +2264,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -2109,7 +2275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
@@ -2117,7 +2283,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -2127,8 +2293,11 @@
       <c r="J62" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AI62" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -2136,7 +2305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -2144,7 +2313,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
@@ -2152,7 +2321,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -2160,7 +2329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -2168,7 +2337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
@@ -2176,7 +2345,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -2187,7 +2356,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -2198,7 +2367,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -2212,7 +2381,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>198</v>
       </c>
@@ -2223,7 +2392,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>198</v>
       </c>
@@ -2234,7 +2403,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>69</v>
       </c>
@@ -2254,7 +2423,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>69</v>
       </c>
@@ -2265,7 +2434,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>69</v>
       </c>
@@ -2276,7 +2445,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>84</v>
       </c>
@@ -2287,7 +2456,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -2306,8 +2475,14 @@
       <c r="AG78" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI78" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>96</v>
       </c>
@@ -2321,7 +2496,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>96</v>
       </c>
@@ -2335,7 +2510,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>96</v>
       </c>
@@ -2346,7 +2521,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
@@ -2360,7 +2535,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>118</v>
       </c>
@@ -2374,7 +2549,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>118</v>
       </c>
@@ -2385,7 +2560,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>118</v>
       </c>
@@ -2398,8 +2573,11 @@
       <c r="AF85" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AJ85" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>118</v>
       </c>
@@ -2413,7 +2591,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>96</v>
       </c>
@@ -2424,7 +2602,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>96</v>
       </c>
@@ -2440,8 +2618,11 @@
       <c r="AF88" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH88" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>96</v>
       </c>
@@ -2457,8 +2638,17 @@
       <c r="AF89" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH89" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AI89" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AJ89" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>96</v>
       </c>
@@ -2474,8 +2664,11 @@
       <c r="AF90" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH90" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>96</v>
       </c>
@@ -2488,8 +2681,11 @@
       <c r="AG91" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="92" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH91" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="92" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -2502,8 +2698,14 @@
       <c r="AF92" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH92" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AJ92" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>84</v>
       </c>
@@ -2514,7 +2716,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>69</v>
       </c>
@@ -2528,7 +2730,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>69</v>
       </c>
@@ -2539,7 +2741,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>69</v>
       </c>
@@ -2550,7 +2752,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>84</v>
       </c>
@@ -2561,7 +2763,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>84</v>
       </c>
@@ -2575,7 +2777,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>96</v>
       </c>
@@ -2584,6 +2786,108 @@
       </c>
       <c r="AF99" s="1" t="s">
         <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B100" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ100" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B101" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="AJ101" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B102" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="AJ102" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B103" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ103" s="11"/>
+    </row>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B104" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ104" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B105" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="AJ105" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B106" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="AJ106" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B107" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AJ107" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B108" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AJ108" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B109" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="AJ109" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B110" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="AJ110" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B111" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="AJ111" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B112" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="AJ112" s="11" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added requirement for lactate synthesis for gf for c parvum
</commit_message>
<xml_diff>
--- a/data/auxotrophies_references.xlsx
+++ b/data/auxotrophies_references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maureencarey/local_documents/work/comparative_parasite_models/paradigm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C20AE-13AC-4C46-95D2-4875CEEE3453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707F627E-9173-1C4A-9220-7967BD092286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="247">
   <si>
     <t>Metabolite</t>
   </si>
@@ -763,6 +763,9 @@
   </si>
   <si>
     <t>tocopherolquinone (alpha)</t>
+  </si>
+  <si>
+    <t>biochem_prod: 10.1371/journal.ppat.1005250</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="X92" sqref="X92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2639,6 +2642,9 @@
       <c r="B91" s="5" t="s">
         <v>107</v>
       </c>
+      <c r="X91" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="AF91" s="1" t="s">
         <v>212</v>
       </c>

</xml_diff>

<commit_message>
added notes to iPfal17 and some auxotrophies
</commit_message>
<xml_diff>
--- a/data/auxotrophies_references.xlsx
+++ b/data/auxotrophies_references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maureencarey/local_documents/work/comparative_parasite_models/paradigm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707F627E-9173-1C4A-9220-7967BD092286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4DB3DB-91FC-3442-A71C-D609835A5441}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24400" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="260">
   <si>
     <t>Metabolite</t>
   </si>
@@ -766,6 +766,45 @@
   </si>
   <si>
     <t>biochem_prod: 10.1371/journal.ppat.1005250</t>
+  </si>
+  <si>
+    <t>braziliensis</t>
+  </si>
+  <si>
+    <t>biochem_uptake: PMID3054535</t>
+  </si>
+  <si>
+    <t>donovani</t>
+  </si>
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t>biochem_prod: PMID3054535</t>
+  </si>
+  <si>
+    <t>L-lactate</t>
+  </si>
+  <si>
+    <t>D-lactate</t>
+  </si>
+  <si>
+    <t>glycerol</t>
+  </si>
+  <si>
+    <t>essential_if_no_glucose: 10.1007/s00436-015-4383-5</t>
+  </si>
+  <si>
+    <t>biochem_uptake: 10.1016/0378-1097(95)00214-P</t>
+  </si>
+  <si>
+    <t>both: biochem_prod: 10.1371/journal.pntd.0001831, biochem_uptake: 10.1016/0378-1097(95)00214-P</t>
+  </si>
+  <si>
+    <t>biochem_prod: 10.1016/0378-1097(95)00214-P</t>
+  </si>
+  <si>
+    <t>both: 10.1016/0378-1097(95)00214-P</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ115"/>
+  <dimension ref="A1:AM118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="X92" sqref="X92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AM22" sqref="AM22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1250,7 +1289,7 @@
     <col min="32" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1354,13 +1393,22 @@
         <v>214</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -1461,16 +1509,25 @@
         <v>202</v>
       </c>
       <c r="AH2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1513,14 +1570,17 @@
       <c r="AG3" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AL3" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM3" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -1538,8 +1598,11 @@
       <c r="AF4" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM4" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -1552,11 +1615,14 @@
       <c r="J5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AL5" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM5" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
@@ -1574,14 +1640,17 @@
       <c r="AF6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AK6" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AL6" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM6" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
@@ -1598,7 +1667,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -1616,11 +1685,11 @@
       <c r="AF8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AK8" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
@@ -1638,11 +1707,14 @@
       <c r="AF9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AH9" s="1" t="s">
+      <c r="AK9" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM9" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
@@ -1656,7 +1728,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -1670,7 +1742,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1685,9 +1757,12 @@
       <c r="AF12" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AI12" s="2"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -1702,9 +1777,12 @@
       <c r="AF13" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AI13" s="2"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -1718,7 +1796,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -1732,7 +1810,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1745,8 +1823,11 @@
       <c r="J16" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM16" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1759,11 +1840,11 @@
       <c r="J17" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AH17" s="1" t="s">
+      <c r="AK17" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -1779,8 +1860,11 @@
       <c r="AF18" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM18" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1793,11 +1877,14 @@
       <c r="J19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AI19" s="1" t="s">
+      <c r="AL19" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM19" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
@@ -1813,11 +1900,11 @@
       <c r="AF20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AJ20" s="11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM20" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1830,8 +1917,11 @@
       <c r="J21" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM21" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1848,7 +1938,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1862,7 +1952,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1873,7 +1963,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -1884,7 +1974,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
@@ -1901,7 +1991,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1918,7 +2008,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1926,7 +2016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1937,7 +2027,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1948,18 +2038,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AJ31" s="11" t="s">
+      <c r="AM31" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1967,7 +2057,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -1977,11 +2067,11 @@
       <c r="O33" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AI33" s="1" t="s">
+      <c r="AL33" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
@@ -1989,7 +2079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
@@ -2009,7 +2099,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>62</v>
       </c>
@@ -2026,7 +2116,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -2034,7 +2124,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -2042,7 +2132,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>62</v>
       </c>
@@ -2050,7 +2140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
@@ -2058,7 +2148,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
@@ -2066,7 +2156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>62</v>
       </c>
@@ -2074,7 +2164,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>61</v>
       </c>
@@ -2094,7 +2184,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -2111,7 +2201,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>61</v>
       </c>
@@ -2128,7 +2218,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>62</v>
       </c>
@@ -2145,7 +2235,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
@@ -2153,7 +2243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>62</v>
       </c>
@@ -2164,7 +2254,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
@@ -2175,7 +2265,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -2183,7 +2273,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -2191,7 +2281,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>61</v>
       </c>
@@ -2202,7 +2292,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -2213,7 +2303,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
@@ -2221,7 +2311,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
@@ -2232,7 +2322,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -2243,7 +2333,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -2257,7 +2347,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -2265,7 +2355,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
@@ -2276,7 +2366,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
@@ -2287,7 +2377,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
@@ -2295,7 +2385,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
@@ -2305,11 +2395,11 @@
       <c r="J62" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AI62" s="1" t="s">
+      <c r="AL62" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
@@ -2317,7 +2407,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
@@ -2489,7 +2579,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -2500,7 +2590,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>92</v>
       </c>
@@ -2520,13 +2610,25 @@
         <v>203</v>
       </c>
       <c r="AH82" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI82" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AJ82" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AK82" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="AI82" s="1" t="s">
+      <c r="AL82" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM82" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>92</v>
       </c>
@@ -2540,7 +2642,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>92</v>
       </c>
@@ -2553,8 +2655,11 @@
       <c r="AF84" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AM84" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>92</v>
       </c>
@@ -2565,7 +2670,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>80</v>
       </c>
@@ -2579,7 +2684,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>114</v>
       </c>
@@ -2593,7 +2698,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>114</v>
       </c>
@@ -2604,7 +2709,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>114</v>
       </c>
@@ -2617,11 +2722,11 @@
       <c r="AF89" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AJ89" s="11" t="s">
+      <c r="AM89" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>114</v>
       </c>
@@ -2635,72 +2740,54 @@
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="X91" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="AF91" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="AH91" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AI91" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ91" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF92" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH92" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="AL92" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
+      </c>
+      <c r="X93" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="AF93" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH93" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AI93" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AJ93" s="11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>209</v>
@@ -2711,224 +2798,287 @@
       <c r="AF94" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AH94" s="1" t="s">
+      <c r="AK94" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="AF95" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG95" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AH95" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK95" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="96" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AL95" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AM95" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>118</v>
       </c>
       <c r="AF96" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK96" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF97" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG97" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK97" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF98" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AH96" s="1" t="s">
+      <c r="AK98" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AJ96" s="11" t="s">
+      <c r="AM98" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B99" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J97" s="1" t="s">
+      <c r="J99" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="J98" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AF98" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="AF99" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF100" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF101" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="AF100" s="1" t="s">
+      <c r="AF102" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B103" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="AG101" s="1" t="s">
+      <c r="AG103" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B104" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="AF102" s="1" t="s">
+      <c r="AF104" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B105" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="AF103" s="1" t="s">
+      <c r="AF105" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B104" s="5" t="s">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B106" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="AJ104" s="1" t="s">
+      <c r="AM106" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B105" s="5" t="s">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B107" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="AJ105" s="1" t="s">
+      <c r="AM107" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B106" s="5" t="s">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B108" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="AJ106" s="1" t="s">
+      <c r="AM108" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B107" s="5" t="s">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B109" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="AJ107" s="11" t="s">
+      <c r="AM109" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B108" s="5" t="s">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B110" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="AJ108" s="11" t="s">
+      <c r="AM110" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B109" s="5" t="s">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B111" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="AJ109" s="11" t="s">
+      <c r="AM111" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B110" s="5" t="s">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="B112" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="AJ110" s="11" t="s">
+      <c r="AM112" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B111" s="5" t="s">
+    <row r="113" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B113" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="AJ111" s="11" t="s">
+      <c r="AM113" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="B112" s="5" t="s">
+    <row r="114" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B114" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="AJ112" s="11" t="s">
+      <c r="AM114" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="113" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B113" s="5" t="s">
+    <row r="115" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B115" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="AJ113" s="11" t="s">
+      <c r="AM115" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B114" s="5" t="s">
+    <row r="116" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B116" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="AJ114" s="11" t="s">
+      <c r="AM116" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="115" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B115" s="5" t="s">
+    <row r="117" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B117" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="AJ115" s="11" t="s">
+      <c r="AM117" s="11" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="118" spans="2:39" x14ac:dyDescent="0.2">
+      <c r="B118" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="AH118" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AI118" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ118" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL118" s="11" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>